<commit_message>
Mejoras del CSS + HTML
</commit_message>
<xml_diff>
--- a/Pruebas unitarias.xlsx
+++ b/Pruebas unitarias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programación\Curso de Python\PROYECTO\fbhub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188FA257-6060-4449-BDAD-167464DBFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A32EF25-D0F8-4CE0-A8B5-E979E8226912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24C2BFEA-A932-4123-A3DD-0B487DAA79DB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -141,7 +141,22 @@
     <t>Cambiar la contraseña y seguir logueado</t>
   </si>
   <si>
-    <t>Cambia la contraseña y sigo logueado</t>
+    <t>Me da el OK y me cambia los datos personales, pero no la contraseña</t>
+  </si>
+  <si>
+    <t>Se actualiza el user_update() para que actualice de manera correcta con el método make_password()</t>
+  </si>
+  <si>
+    <t>Cambia la contraseña y desloguea</t>
+  </si>
+  <si>
+    <t>Se agrega la advertencia al cliente indicando que se va a pedir que se loguee nuevamente por motivos de seguridad</t>
+  </si>
+  <si>
+    <t>Cambiar la contraseña y desloguear pidiendo logueo nuevamente</t>
+  </si>
+  <si>
+    <t>Cambia contraseña y desloguea</t>
   </si>
 </sst>
 </file>
@@ -232,14 +247,14 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF00B050"/>
+        <color rgb="FFFF0000"/>
       </font>
     </dxf>
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
       </font>
     </dxf>
     <dxf>
@@ -569,7 +584,7 @@
   <dimension ref="A2:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,7 +799,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="H9" s="3">
         <v>7</v>
       </c>
@@ -801,33 +816,57 @@
         <v>38</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="H10" s="3">
         <v>8</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I10" s="5">
+        <v>44994</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="H11" s="3">
         <v>9</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
+      <c r="I11" s="5">
+        <v>44994</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H12" s="3">
@@ -853,10 +892,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"SI"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Se añade funcionalidad de comentarios
</commit_message>
<xml_diff>
--- a/Pruebas unitarias.xlsx
+++ b/Pruebas unitarias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programación\Curso de Python\PROYECTO\fbhub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A32EF25-D0F8-4CE0-A8B5-E979E8226912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD63284-6B65-479C-9A8B-BE18E98EBABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24C2BFEA-A932-4123-A3DD-0B487DAA79DB}"/>
+    <workbookView xWindow="3180" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{24C2BFEA-A932-4123-A3DD-0B487DAA79DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -157,22 +157,44 @@
   </si>
   <si>
     <t>Cambia contraseña y desloguea</t>
+  </si>
+  <si>
+    <t>Intento agregar un comentario con la funcionalidad recientemente agregada</t>
+  </si>
+  <si>
+    <t>Genera comentario y devuelve a Inicio</t>
+  </si>
+  <si>
+    <t>ValueError</t>
+  </si>
+  <si>
+    <t>Se debuguea en varias medidas el HTML, la URL, la view y se relaciona uno a uno la clase de comentarios para poder identificar cualquier objeto que se le brinda</t>
+  </si>
+  <si>
+    <t>Intento agregar un comentario a un objeto de cualquiera de las clases</t>
+  </si>
+  <si>
+    <t>Genera comentario</t>
+  </si>
+  <si>
+    <t>Genera comentario OK</t>
+  </si>
+  <si>
+    <t>Eliminar comentario y quedarse en la página</t>
+  </si>
+  <si>
+    <t>Elimina comentario OK</t>
+  </si>
+  <si>
+    <t>Intento eliminar un comentario propio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -221,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,9 +252,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -581,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8FB4FF-8A3D-4089-ADE5-E164AFC9CCEB}">
-  <dimension ref="A2:N13"/>
+  <dimension ref="A2:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +672,7 @@
       <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>44992</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -688,7 +707,7 @@
       <c r="H4" s="3">
         <v>2</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>44992</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -711,7 +730,7 @@
       <c r="H5" s="3">
         <v>3</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="4">
         <v>44993</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -734,7 +753,7 @@
       <c r="H6" s="3">
         <v>4</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>44993</v>
       </c>
       <c r="J6" s="3" t="s">
@@ -757,7 +776,7 @@
       <c r="H7" s="3">
         <v>5</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>44993</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -780,7 +799,7 @@
       <c r="H8" s="3">
         <v>6</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>44994</v>
       </c>
       <c r="J8" s="3" t="s">
@@ -803,7 +822,7 @@
       <c r="H9" s="3">
         <v>7</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>44994</v>
       </c>
       <c r="J9" s="3" t="s">
@@ -826,7 +845,7 @@
       <c r="H10" s="3">
         <v>8</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>44994</v>
       </c>
       <c r="J10" s="3" t="s">
@@ -849,7 +868,7 @@
       <c r="H11" s="3">
         <v>9</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>44994</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -868,22 +887,230 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="H12" s="3">
         <v>10</v>
       </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M13" s="4"/>
+      <c r="I12" s="4">
+        <v>44995</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="3">
+        <v>11</v>
+      </c>
+      <c r="I13" s="4">
+        <v>44995</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="3">
+        <v>12</v>
+      </c>
+      <c r="I14" s="4">
+        <v>44995</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H15" s="3"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H19" s="3"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H20" s="3"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H21" s="3"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H22" s="3"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H23" s="3"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H25" s="3"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H27" s="3"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H28" s="3"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H30" s="3"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H31" s="3"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="M3:M8 M10:M1048576">
+  <conditionalFormatting sqref="M3:M1048576">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>

</xml_diff>